<commit_message>
#1 - Started bit on program and updated risk assessment
</commit_message>
<xml_diff>
--- a/requirements gathering/IC-IT-Risk-Assessment-Matrix-Template-8849.xlsx
+++ b/requirements gathering/IC-IT-Risk-Assessment-Matrix-Template-8849.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\premal\Google Drive\QAC projects\Email-automation-for-Tobor-users\requirements gathering\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DA31FDD-9368-4636-A90A-20D6AAE04ED4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADF9F03A-DB47-4326-94C6-6E25696AAD23}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19080" yWindow="-120" windowWidth="24240" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21210" yWindow="3435" windowWidth="14400" windowHeight="10755" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IT Risk Assessment Matrix" sheetId="4" r:id="rId1"/>
@@ -1502,7 +1502,7 @@
       <c r="K18" s="20"/>
     </row>
     <row r="19" spans="2:11" ht="10.15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="2:11" ht="49.9" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:11" ht="49.9" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B20" s="28" t="s">
         <v>26</v>
       </c>

</xml_diff>